<commit_message>
inclusao da analise xls
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_P01_.xlsx
+++ b/Experiment01_Resumo/Resumo_P01_.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
     <sheet name="Resumo DatabaseSnowballing" sheetId="8" r:id="rId2"/>
     <sheet name="SearchResults" sheetId="9" r:id="rId3"/>
     <sheet name="Seed Set" sheetId="5" r:id="rId4"/>
-    <sheet name="Scopus" sheetId="10" r:id="rId5"/>
-    <sheet name="Plan2" sheetId="12" r:id="rId6"/>
-    <sheet name="RQ" sheetId="11" r:id="rId7"/>
+    <sheet name="RQ" sheetId="11" r:id="rId5"/>
+    <sheet name="Scopus" sheetId="10" r:id="rId6"/>
+    <sheet name="Plan2" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="287">
   <si>
     <t>Database search</t>
   </si>
@@ -836,30 +836,7 @@
     <t xml:space="preserve">Paper Name </t>
   </si>
   <si>
-    <t>Research Question 1) Qual das bibliotecas digitais é mais eficiente?</t>
-  </si>
-  <si>
-    <t>A estratégia híbrida envolve analisar menos artigos quando comparada com as SLRs publicadas que conduziram buscas somente em bases de dados? Precision
-A estratégia híbrida recupera todos os artigos que estavam incluídos na SLR publicada que conduziu as buscas em bases de dados? Recall.</t>
-  </si>
-  <si>
     <t>Biblioteca Digital</t>
-  </si>
-  <si>
-    <t>Precision</t>
-  </si>
-  <si>
-    <t>Recall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/22 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/17 = </t>
-  </si>
-  <si>
-    <t>RQ1) Qual busca em biblioteca digital encontra mais artigos incluídos na lista de selecionados da SLR publicada dentre o resultado retornado na busca?
-RQ2) Qual busca em biblioteca digital recupera todos os artigos que estavam incluídos na lista de selecionados da SRL publicada?</t>
   </si>
   <si>
     <t>Ameaça à validade: 1) a busca que realizo limitada a 2015, no forward temos somente busca por filtro de até o ano de 2015. No primeiro backward, pode ser que seja eliminada alguma referencia retornada na busca e não lida. 2) As estrategias estão em loop com o repeat. 3) 
@@ -869,6 +846,128 @@
     <t>1) um artigo de 2017 cita no forward um de 2015. Deve ser selecionado?
 2) Artigos selecionados no forward deveriam ser somente em ingles; Existem em russo, espanhol, japones.
 3) Tese deveria ser selecionada? Qual critério? 4)No forward de  albuquerque2009a tivemos 5 artigos( 4 existentes e 1 incluído), como eu visualizo essa informação?</t>
+  </si>
+  <si>
+    <t>JF tool</t>
+  </si>
+  <si>
+    <t>Qtd Ref encontrado no Scopus</t>
+  </si>
+  <si>
+    <t>0/128= 0</t>
+  </si>
+  <si>
+    <t>0/22=0</t>
+  </si>
+  <si>
+    <t>RQ1.1) Qual busca em biblioteca digital encontra mais artigos incluídos na lista de selecionados da SLR publicada dentre o resultado retornado na busca?
+RQ1.2) Qual busca em biblioteca digital recupera todos os artigos que estavam incluídos na lista de selecionados da SRL publicada?</t>
+  </si>
+  <si>
+    <t>Research Question 1) Qual das bibliotecas digitais utilizadas na SLR publicada é mais eficiente?</t>
+  </si>
+  <si>
+    <t>Research Questions</t>
+  </si>
+  <si>
+    <t>7/16= 43%</t>
+  </si>
+  <si>
+    <t>5/10= 50%</t>
+  </si>
+  <si>
+    <t>1/182= 0,5%</t>
+  </si>
+  <si>
+    <t>1/103= 0,98%</t>
+  </si>
+  <si>
+    <t>7/22= 31,8%</t>
+  </si>
+  <si>
+    <t>5/22= 22,7%</t>
+  </si>
+  <si>
+    <t>1/22= 4,5%</t>
+  </si>
+  <si>
+    <t>RQ2.1)A estratégia híbrida envolve analisar menos artigos quando comparada com as SLRs publicadas que conduziram buscas somente em bases de dados? Precision
+RQ2.2)A estratégia híbrida recupera todos os artigos que estavam incluídos na SLR publicada que conduziu as buscas em bases de dados? Recall.</t>
+  </si>
+  <si>
+    <t>Busca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snowballing </t>
+  </si>
+  <si>
+    <t>Guideline 2014</t>
+  </si>
+  <si>
+    <t>Short Paper 2017</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>Google Scholar</t>
+  </si>
+  <si>
+    <t>Código Snowballing</t>
+  </si>
+  <si>
+    <t>ID Estratégia</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>Todas Bibliotecas Digitais</t>
+  </si>
+  <si>
+    <t>Estratégia Somente Busca</t>
+  </si>
+  <si>
+    <t>SFBU</t>
+  </si>
+  <si>
+    <t>S2FFBB2U</t>
+  </si>
+  <si>
+    <t>BBFF</t>
+  </si>
+  <si>
+    <t>FFBB</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>Estratégia Híbrida (Busca + Snowballing)</t>
+  </si>
+  <si>
+    <t>Research Question 3) Qual das estratégias é mais eficiente?</t>
+  </si>
+  <si>
+    <t>Research Question 2) Qual das estratégias híbridas é mais eficiente?</t>
+  </si>
+  <si>
+    <t>JF new BF 2018</t>
+  </si>
+  <si>
+    <t>JF new FB 2018</t>
   </si>
 </sst>
 </file>
@@ -1013,12 +1112,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1065,8 +1158,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1327,68 +1426,103 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1398,7 +1532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1512,35 +1646,14 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1561,22 +1674,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1586,7 +1699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1605,10 +1718,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1639,16 +1752,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1657,27 +1770,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1735,38 +1827,89 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2062,22 +2205,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="117"/>
+      <c r="B1" s="101"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="119"/>
+      <c r="B2" s="103"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="119"/>
+      <c r="B3" s="103"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -2112,10 +2255,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="121"/>
+      <c r="B8" s="105"/>
     </row>
     <row r="9" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -2195,10 +2338,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="110" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="127"/>
+      <c r="B1" s="111"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
@@ -2231,16 +2374,16 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="107"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="108" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="125"/>
+      <c r="B7" s="109"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
@@ -2304,8 +2447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,17 +2466,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="112" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="130"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="114"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
     </row>
@@ -2696,8 +2839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2708,19 +2851,21 @@
     <col min="4" max="4" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.5703125" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>125</v>
       </c>
@@ -2738,6 +2883,9 @@
       </c>
       <c r="F2" s="29" t="s">
         <v>148</v>
+      </c>
+      <c r="G2" s="132" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2759,9 +2907,10 @@
       <c r="F3" s="7">
         <v>25</v>
       </c>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="31" t="s">
@@ -2779,12 +2928,12 @@
       <c r="F4" s="7">
         <v>20</v>
       </c>
-      <c r="G4" s="103">
+      <c r="G4" s="96">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -2802,12 +2951,12 @@
       <c r="F5" s="7">
         <v>24</v>
       </c>
-      <c r="G5" s="103">
+      <c r="G5" s="96">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -2825,10 +2974,10 @@
       <c r="F6" s="7">
         <v>57</v>
       </c>
-      <c r="G6" s="103"/>
+      <c r="G6" s="96"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="33" t="s">
@@ -2846,12 +2995,12 @@
       <c r="F7" s="5">
         <v>11</v>
       </c>
-      <c r="G7" s="80">
+      <c r="G7" s="73">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="33" t="s">
@@ -2869,7 +3018,7 @@
       <c r="F8" s="5">
         <v>22</v>
       </c>
-      <c r="G8" s="80"/>
+      <c r="G8" s="73"/>
     </row>
     <row r="9" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -2890,9 +3039,10 @@
       <c r="F9" s="5">
         <v>13</v>
       </c>
+      <c r="G9" s="70"/>
     </row>
     <row r="10" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2910,7 +3060,7 @@
       <c r="F10" s="5">
         <v>43</v>
       </c>
-      <c r="G10" s="80">
+      <c r="G10" s="73">
         <v>43</v>
       </c>
     </row>
@@ -2933,6 +3083,7 @@
       <c r="F11" s="5">
         <v>11</v>
       </c>
+      <c r="G11" s="70"/>
     </row>
     <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -2953,6 +3104,7 @@
       <c r="F12" s="6">
         <v>37</v>
       </c>
+      <c r="G12" s="70"/>
     </row>
     <row r="13" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -2973,9 +3125,10 @@
       <c r="F13" s="5">
         <v>16</v>
       </c>
+      <c r="G13" s="70"/>
     </row>
     <row r="14" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="33" t="s">
@@ -2993,12 +3146,12 @@
       <c r="F14" s="5">
         <v>14</v>
       </c>
-      <c r="G14" s="80">
+      <c r="G14" s="73">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="33" t="s">
@@ -3016,12 +3169,12 @@
       <c r="F15" s="5">
         <v>8</v>
       </c>
-      <c r="G15" s="80">
+      <c r="G15" s="73">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="33" t="s">
@@ -3039,12 +3192,12 @@
       <c r="F16" s="5">
         <v>27</v>
       </c>
-      <c r="G16" s="80">
+      <c r="G16" s="73">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="33" t="s">
@@ -3062,7 +3215,7 @@
       <c r="F17" s="5">
         <v>14</v>
       </c>
-      <c r="G17" s="80">
+      <c r="G17" s="73">
         <v>14</v>
       </c>
     </row>
@@ -3085,9 +3238,10 @@
       <c r="F18" s="5">
         <v>8</v>
       </c>
+      <c r="G18" s="70"/>
     </row>
     <row r="19" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -3105,10 +3259,10 @@
       <c r="F19" s="5">
         <v>15</v>
       </c>
-      <c r="G19" s="104"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -3126,7 +3280,7 @@
       <c r="F20" s="5">
         <v>18</v>
       </c>
-      <c r="G20" s="104"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
@@ -3147,9 +3301,10 @@
       <c r="F21" s="5">
         <v>22</v>
       </c>
+      <c r="G21" s="70"/>
     </row>
     <row r="22" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -3167,7 +3322,7 @@
       <c r="F22" s="5">
         <v>15</v>
       </c>
-      <c r="G22" s="104"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -3188,6 +3343,7 @@
       <c r="F23" s="5">
         <v>11</v>
       </c>
+      <c r="G23" s="70"/>
     </row>
     <row r="24" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
@@ -3208,6 +3364,7 @@
       <c r="F24" s="5">
         <v>33</v>
       </c>
+      <c r="G24" s="70"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
@@ -3217,7 +3374,7 @@
         <f>SUM(F3:F24)</f>
         <v>464</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="70">
         <f>SUM(G3:G24)</f>
         <v>161</v>
       </c>
@@ -3235,7 +3392,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3243,712 +3400,1195 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView topLeftCell="E9" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="134" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="136" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="136"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+    </row>
+    <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="137" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133"/>
+      <c r="O3" s="133"/>
+      <c r="P3" s="133"/>
+      <c r="Q3" s="133"/>
+      <c r="R3" s="133"/>
+      <c r="S3" s="133"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="141" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
+    </row>
+    <row r="5" spans="1:19" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="99" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" s="99" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="99" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" s="99" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="138" t="s">
+        <v>274</v>
+      </c>
+      <c r="N6" s="38"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>250</v>
+      </c>
+      <c r="D7" s="139"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="139"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="139"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="74" t="s">
+        <v>260</v>
+      </c>
+      <c r="D10" s="139"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" s="74" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" s="139"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="140"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="136" t="s">
+        <v>284</v>
+      </c>
+      <c r="B13" s="136"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="136"/>
+      <c r="G13" s="136"/>
+      <c r="H13" s="136"/>
+      <c r="I13" s="136"/>
+    </row>
+    <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="137" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14" s="137"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="137"/>
+      <c r="E14" s="137"/>
+      <c r="F14" s="137"/>
+      <c r="G14" s="137"/>
+      <c r="H14" s="137"/>
+      <c r="I14" s="137"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="133"/>
+      <c r="L14" s="133"/>
+      <c r="M14" s="133"/>
+      <c r="N14" s="133"/>
+      <c r="O14" s="133"/>
+      <c r="P14" s="133"/>
+      <c r="Q14" s="133"/>
+      <c r="R14" s="133"/>
+      <c r="S14" s="133"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="142" t="s">
+        <v>282</v>
+      </c>
+      <c r="B15" s="141"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="141"/>
+      <c r="E15" s="141"/>
+      <c r="F15" s="141"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="99" t="s">
+        <v>262</v>
+      </c>
+      <c r="B16" s="99" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="99" t="s">
+        <v>272</v>
+      </c>
+      <c r="D16" s="99" t="s">
+        <v>273</v>
+      </c>
+      <c r="E16" s="99" t="s">
+        <v>210</v>
+      </c>
+      <c r="F16" s="99" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="87" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="74" t="s">
+        <v>277</v>
+      </c>
+      <c r="D17" s="74" t="s">
+        <v>281</v>
+      </c>
+      <c r="E17" s="143"/>
+      <c r="F17" s="143"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="C18" s="74" t="s">
+        <v>277</v>
+      </c>
+      <c r="D18" s="74" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>277</v>
+      </c>
+      <c r="D19" s="74" t="s">
+        <v>267</v>
+      </c>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="70" t="s">
+        <v>265</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>278</v>
+      </c>
+      <c r="D20" s="74" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="C21" s="74" t="s">
+        <v>279</v>
+      </c>
+      <c r="D21" s="74" t="s">
+        <v>269</v>
+      </c>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="70" t="s">
+        <v>286</v>
+      </c>
+      <c r="C22" s="74" t="s">
+        <v>280</v>
+      </c>
+      <c r="D22" s="74" t="s">
+        <v>270</v>
+      </c>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="136" t="s">
+        <v>283</v>
+      </c>
+      <c r="B23" s="136"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="136"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="136"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="136"/>
+    </row>
+    <row r="24" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="137" t="s">
+        <v>261</v>
+      </c>
+      <c r="B24" s="137"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="137"/>
+      <c r="G24" s="137"/>
+      <c r="H24" s="137"/>
+      <c r="I24" s="137"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="99" t="s">
+        <v>273</v>
+      </c>
+      <c r="B25" s="99" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="99" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="B26" s="143"/>
+      <c r="C26" s="143"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="74" t="s">
+        <v>281</v>
+      </c>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="74" t="s">
+        <v>266</v>
+      </c>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="74" t="s">
+        <v>267</v>
+      </c>
+      <c r="B29" s="70"/>
+      <c r="C29" s="70"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="74" t="s">
+        <v>268</v>
+      </c>
+      <c r="B30" s="70"/>
+      <c r="C30" s="70"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="74" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="74" t="s">
+        <v>270</v>
+      </c>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A4:D4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="34" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="131" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-    </row>
-    <row r="2" spans="1:14" ht="159" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="138" t="s">
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+    </row>
+    <row r="2" spans="1:14" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="124" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="72" t="s">
         <v>184</v>
       </c>
-      <c r="D4" s="112" t="s">
+      <c r="D4" s="72" t="s">
         <v>185</v>
       </c>
-      <c r="E4" s="112" t="s">
+      <c r="E4" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="72" t="s">
         <v>220</v>
       </c>
-      <c r="G4" s="79" t="s">
+      <c r="G4" s="72" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="H4" s="72" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="58" t="s">
+      <c r="B5" s="53"/>
+      <c r="C5" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="31" t="s">
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="78" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="H5" s="74"/>
+    </row>
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="59" t="s">
+      <c r="B6" s="53"/>
+      <c r="C6" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="77">
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74">
         <v>20</v>
       </c>
-      <c r="G6" s="105" t="s">
+      <c r="G6" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="108" t="s">
+      <c r="H6" s="129" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+    <row r="7" spans="1:14" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="59" t="s">
+      <c r="B7" s="53"/>
+      <c r="C7" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="77">
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74">
         <v>24</v>
       </c>
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="109" t="s">
+      <c r="H7" s="130" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58" t="s">
+      <c r="B8" s="53"/>
+      <c r="C8" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="32" t="s">
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="78" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="H8" s="74"/>
+    </row>
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="59" t="s">
+      <c r="B9" s="53"/>
+      <c r="C9" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="77">
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74">
         <v>11</v>
       </c>
-      <c r="G9" s="106" t="s">
+      <c r="G9" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="110" t="s">
+      <c r="H9" s="129" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58" t="s">
+      <c r="B10" s="53"/>
+      <c r="C10" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="55"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="94" t="s">
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="78" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="H10" s="74"/>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58" t="s">
+      <c r="B11" s="53"/>
+      <c r="C11" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="55"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="94" t="s">
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" s="53" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+      <c r="H11" s="74"/>
+    </row>
+    <row r="12" spans="1:14" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="59" t="s">
+      <c r="B12" s="53"/>
+      <c r="C12" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="111">
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="125">
         <v>44</v>
       </c>
-      <c r="G12" s="107" t="s">
+      <c r="G12" s="128" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="110" t="s">
+      <c r="H12" s="129" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="58" t="s">
+      <c r="B13" s="53"/>
+      <c r="C13" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="94" t="s">
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="78" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="H13" s="74"/>
+    </row>
+    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="58" t="s">
+      <c r="B14" s="53"/>
+      <c r="C14" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="94" t="s">
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="78" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="H14" s="74"/>
+    </row>
+    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58" t="s">
+      <c r="B15" s="53"/>
+      <c r="C15" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="94" t="s">
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="78" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="H15" s="74"/>
+    </row>
+    <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="59" t="s">
+      <c r="B16" s="53"/>
+      <c r="C16" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="77">
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74">
         <v>14</v>
       </c>
-      <c r="G16" s="106" t="s">
+      <c r="G16" s="128" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="110" t="s">
+      <c r="H16" s="129" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="s">
+    <row r="17" spans="1:11" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="59" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="55"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="77">
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74">
         <v>8</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="110" t="s">
+      <c r="H17" s="129" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="59" t="s">
+      <c r="B18" s="53"/>
+      <c r="C18" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="77">
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74">
         <v>27</v>
       </c>
-      <c r="G18" s="106" t="s">
+      <c r="G18" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="110" t="s">
+      <c r="H18" s="129" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+    <row r="19" spans="1:11" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="59" t="s">
+      <c r="B19" s="53"/>
+      <c r="C19" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="55"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="77">
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74">
         <v>14</v>
       </c>
-      <c r="G19" s="106" t="s">
+      <c r="G19" s="128" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="110" t="s">
+      <c r="H19" s="129" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="58" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="94" t="s">
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="78" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="57" t="s">
+      <c r="H20" s="74"/>
+    </row>
+    <row r="21" spans="1:11" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="58" t="s">
+      <c r="B21" s="53"/>
+      <c r="C21" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="8" t="s">
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="78" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="57" t="s">
+      <c r="H21" s="74"/>
+    </row>
+    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="58" t="s">
+      <c r="B22" s="53"/>
+      <c r="C22" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="8" t="s">
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="78" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
+      <c r="H22" s="74"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="58" t="s">
+      <c r="B23" s="53"/>
+      <c r="C23" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="8" t="s">
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="78" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="57" t="s">
+      <c r="H23" s="74"/>
+    </row>
+    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="58" t="s">
+      <c r="B24" s="53"/>
+      <c r="C24" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="55"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="8" t="s">
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="78" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="H24" s="74"/>
+    </row>
+    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="58" t="s">
+      <c r="B25" s="53"/>
+      <c r="C25" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="8" t="s">
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="78" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
+      <c r="H25" s="74"/>
+    </row>
+    <row r="26" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="58" t="s">
+      <c r="B26" s="53"/>
+      <c r="C26" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="55"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="8" t="s">
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="78" t="s">
         <v>92</v>
       </c>
+      <c r="H26" s="74"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F27" s="106">
+      <c r="A27" s="74"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="126">
         <f>SUM(F5:F26)</f>
         <v>162</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" s="76" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="82"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+    </row>
+    <row r="28" spans="1:11" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="75"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="133" t="s">
+      <c r="A29" s="119" t="s">
         <v>189</v>
       </c>
-      <c r="B29" s="133"/>
-      <c r="C29" s="133"/>
-      <c r="D29" s="75"/>
-      <c r="F29" s="69" t="s">
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="68"/>
+      <c r="I29" s="118" t="s">
+        <v>205</v>
+      </c>
+      <c r="J29" s="118"/>
+      <c r="K29" s="118"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="120" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="120"/>
+      <c r="C30" s="74" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" s="71"/>
+      <c r="I30" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="J30" s="74">
+        <v>17</v>
+      </c>
+      <c r="K30" s="86"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="120" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" s="120"/>
+      <c r="C31" s="82" t="s">
+        <v>239</v>
+      </c>
+      <c r="D31" s="71"/>
+      <c r="I31" s="77" t="s">
+        <v>207</v>
+      </c>
+      <c r="J31" s="74">
+        <v>22</v>
+      </c>
+      <c r="K31" s="73"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="120" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="120"/>
+      <c r="C32" s="82" t="s">
+        <v>240</v>
+      </c>
+      <c r="D32" s="71"/>
+      <c r="I32" s="84" t="s">
+        <v>218</v>
+      </c>
+      <c r="J32" s="73">
+        <v>8</v>
+      </c>
+      <c r="K32" s="73"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="116" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" s="116"/>
+      <c r="C33" s="117" t="s">
+        <v>231</v>
+      </c>
+      <c r="D33" s="98"/>
+      <c r="I33" s="84" t="s">
+        <v>208</v>
+      </c>
+      <c r="J33" s="73">
+        <v>14</v>
+      </c>
+      <c r="K33" s="73"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="116"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="98"/>
+      <c r="I34" s="83" t="s">
+        <v>185</v>
+      </c>
+      <c r="J34" s="88" t="s">
+        <v>237</v>
+      </c>
+      <c r="K34" s="74"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I35" s="83" t="s">
+        <v>186</v>
+      </c>
+      <c r="J35" s="88" t="s">
+        <v>238</v>
+      </c>
+      <c r="K35" s="74"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I36" s="85"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I37" s="80" t="s">
+        <v>209</v>
+      </c>
+      <c r="J37" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="K37" s="79" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I38" s="93" t="s">
+        <v>212</v>
+      </c>
+      <c r="J38" s="78" t="s">
+        <v>219</v>
+      </c>
+      <c r="K38" s="81" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I39" s="92" t="s">
+        <v>213</v>
+      </c>
+      <c r="J39" s="88" t="s">
+        <v>236</v>
+      </c>
+      <c r="K39" s="82" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I40" s="92" t="s">
+        <v>214</v>
+      </c>
+      <c r="J40" s="88" t="s">
+        <v>230</v>
+      </c>
+      <c r="K40" s="82" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I41" s="91" t="s">
+        <v>216</v>
+      </c>
+      <c r="J41" s="89" t="s">
+        <v>235</v>
+      </c>
+      <c r="K41" s="82" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I42" s="94" t="s">
+        <v>217</v>
+      </c>
+      <c r="J42" s="90" t="s">
+        <v>241</v>
+      </c>
+      <c r="K42" s="74" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="I44" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="J44" s="97" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I47" s="62" t="s">
         <v>193</v>
       </c>
-      <c r="G29" s="61" t="s">
+      <c r="J47" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="I29" s="132" t="s">
-        <v>205</v>
-      </c>
-      <c r="J29" s="132"/>
-      <c r="K29" s="132"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="135" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="135"/>
-      <c r="C30" s="81" t="s">
-        <v>204</v>
-      </c>
-      <c r="D30" s="78"/>
-      <c r="F30" s="70" t="s">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I48" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="G30" s="62">
+      <c r="J48" s="55">
         <v>22</v>
       </c>
-      <c r="I30" s="84" t="s">
-        <v>206</v>
-      </c>
-      <c r="J30" s="81">
-        <v>17</v>
-      </c>
-      <c r="K30" s="93"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="135" t="s">
-        <v>190</v>
-      </c>
-      <c r="B31" s="135"/>
-      <c r="C31" s="89" t="s">
-        <v>239</v>
-      </c>
-      <c r="D31" s="78"/>
-      <c r="F31" s="71" t="s">
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="64" t="s">
         <v>196</v>
       </c>
-      <c r="G31" s="63">
+      <c r="J49" s="56">
         <v>8</v>
       </c>
-      <c r="I31" s="84" t="s">
-        <v>207</v>
-      </c>
-      <c r="J31" s="81">
-        <v>22</v>
-      </c>
-      <c r="K31" s="80"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="135" t="s">
-        <v>191</v>
-      </c>
-      <c r="B32" s="135"/>
-      <c r="C32" s="89" t="s">
-        <v>240</v>
-      </c>
-      <c r="D32" s="78"/>
-      <c r="F32" s="70" t="s">
+    </row>
+    <row r="50" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="63" t="s">
         <v>197</v>
       </c>
-      <c r="G32" s="62">
+      <c r="J50" s="55">
         <v>14</v>
       </c>
-      <c r="I32" s="91" t="s">
-        <v>218</v>
-      </c>
-      <c r="J32" s="80">
-        <v>8</v>
-      </c>
-      <c r="K32" s="80"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="136" t="s">
-        <v>192</v>
-      </c>
-      <c r="B33" s="136"/>
-      <c r="C33" s="137" t="s">
-        <v>231</v>
-      </c>
-      <c r="D33" s="114"/>
-      <c r="F33" s="71" t="s">
+    </row>
+    <row r="51" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="64" t="s">
         <v>198</v>
       </c>
-      <c r="G33" s="63" t="s">
+      <c r="J51" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="I33" s="91" t="s">
-        <v>208</v>
-      </c>
-      <c r="J33" s="80">
-        <v>14</v>
-      </c>
-      <c r="K33" s="80"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="136"/>
-      <c r="B34" s="136"/>
-      <c r="C34" s="137"/>
-      <c r="D34" s="114"/>
-      <c r="F34" s="70" t="s">
+    </row>
+    <row r="52" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="63" t="s">
         <v>199</v>
       </c>
-      <c r="G34" s="64">
+      <c r="J52" s="57">
         <v>12</v>
       </c>
-      <c r="I34" s="90" t="s">
-        <v>185</v>
-      </c>
-      <c r="J34" s="95" t="s">
-        <v>237</v>
-      </c>
-      <c r="K34" s="81"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F35" s="71" t="s">
+    </row>
+    <row r="53" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="64" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="65">
+      <c r="J53" s="58">
         <v>0</v>
       </c>
-      <c r="I35" s="90" t="s">
-        <v>186</v>
-      </c>
-      <c r="J35" s="95" t="s">
-        <v>238</v>
-      </c>
-      <c r="K35" s="81"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F36" s="70" t="s">
+    </row>
+    <row r="54" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="G36" s="66"/>
-      <c r="I36" s="92"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F37" s="72" t="s">
+      <c r="J54" s="59"/>
+    </row>
+    <row r="55" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I55" s="65" t="s">
         <v>202</v>
       </c>
-      <c r="G37" s="67">
+      <c r="J55" s="60">
         <v>10</v>
       </c>
-      <c r="I37" s="87" t="s">
-        <v>209</v>
-      </c>
-      <c r="J37" s="86" t="s">
-        <v>210</v>
-      </c>
-      <c r="K37" s="86" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F38" s="73" t="s">
+    </row>
+    <row r="56" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I56" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="G38" s="68">
+      <c r="J56" s="61">
         <v>12</v>
-      </c>
-      <c r="I38" s="100" t="s">
-        <v>212</v>
-      </c>
-      <c r="J38" s="85" t="s">
-        <v>219</v>
-      </c>
-      <c r="K38" s="88" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I39" s="99" t="s">
-        <v>213</v>
-      </c>
-      <c r="J39" s="95" t="s">
-        <v>236</v>
-      </c>
-      <c r="K39" s="89" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I40" s="99" t="s">
-        <v>214</v>
-      </c>
-      <c r="J40" s="95" t="s">
-        <v>230</v>
-      </c>
-      <c r="K40" s="89" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I41" s="98" t="s">
-        <v>216</v>
-      </c>
-      <c r="J41" s="96" t="s">
-        <v>235</v>
-      </c>
-      <c r="K41" s="89" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I42" s="101" t="s">
-        <v>217</v>
-      </c>
-      <c r="J42" s="97" t="s">
-        <v>241</v>
-      </c>
-      <c r="K42" s="81" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="I44" s="102" t="s">
-        <v>232</v>
-      </c>
-      <c r="J44" s="113" t="s">
-        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3959,22 +4599,22 @@
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A3:G3"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A3:H3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3983,177 +4623,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>252</v>
+      <c r="A1" s="51" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
-        <v>253</v>
+      <c r="A4" s="95" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="142" t="s">
-        <v>251</v>
-      </c>
-      <c r="B3" s="142"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="142"/>
-      <c r="L3" s="142"/>
-      <c r="M3" s="142"/>
-      <c r="N3" s="142"/>
-      <c r="O3" s="142"/>
-      <c r="P3" s="142"/>
-      <c r="Q3" s="142"/>
-      <c r="R3" s="142"/>
-      <c r="S3" s="142"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="142"/>
-      <c r="B4" s="142"/>
-      <c r="C4" s="142"/>
-      <c r="D4" s="142"/>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
-      <c r="G4" s="142"/>
-      <c r="H4" s="142"/>
-      <c r="I4" s="142"/>
-      <c r="J4" s="142"/>
-      <c r="K4" s="142"/>
-      <c r="L4" s="142"/>
-      <c r="M4" s="142"/>
-      <c r="N4" s="142"/>
-      <c r="O4" s="142"/>
-      <c r="P4" s="142"/>
-      <c r="Q4" s="142"/>
-      <c r="R4" s="142"/>
-      <c r="S4" s="142"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="115" t="s">
-        <v>246</v>
-      </c>
-      <c r="B6" s="115" t="s">
-        <v>247</v>
-      </c>
-      <c r="C6" s="115" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="81" t="s">
-        <v>250</v>
-      </c>
-      <c r="C7" s="81" t="s">
-        <v>249</v>
-      </c>
-      <c r="N7" s="38"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="77" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="142" t="s">
-        <v>245</v>
-      </c>
-      <c r="B15" s="142"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="142"/>
-      <c r="E15" s="142"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="142"/>
-      <c r="H15" s="142"/>
-      <c r="I15" s="142"/>
-      <c r="J15" s="142"/>
-      <c r="K15" s="142"/>
-      <c r="L15" s="142"/>
-      <c r="M15" s="142"/>
-      <c r="N15" s="142"/>
-      <c r="O15" s="142"/>
-      <c r="P15" s="142"/>
-      <c r="Q15" s="142"/>
-      <c r="R15" s="142"/>
-      <c r="S15" s="142"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A3:S4"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
inclusao do google scholar
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_P01_.xlsx
+++ b/Experiment01_Resumo/Resumo_P01_.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
     <sheet name="Resumo DatabaseSnowballing" sheetId="8" r:id="rId2"/>
     <sheet name="SearchResults" sheetId="9" r:id="rId3"/>
     <sheet name="Seed Set" sheetId="5" r:id="rId4"/>
-    <sheet name="RQ" sheetId="11" r:id="rId5"/>
+    <sheet name="ResearchQuestions" sheetId="11" r:id="rId5"/>
     <sheet name="Scopus" sheetId="10" r:id="rId6"/>
-    <sheet name="Plan2" sheetId="12" r:id="rId7"/>
+    <sheet name="GoogleScholar" sheetId="13" r:id="rId7"/>
+    <sheet name="Threats" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="301">
   <si>
     <t>Database search</t>
   </si>
@@ -102,9 +103,6 @@
   </si>
   <si>
     <t>Science Direct</t>
-  </si>
-  <si>
-    <t>Publisher</t>
   </si>
   <si>
     <t>S1</t>
@@ -585,9 +583,6 @@
     <t xml:space="preserve">TITLE-ABS-KEY(("software process improvement") AND ("business goal" OR "strategic" OR "goal oriented" OR "business oriented" OR "business strategy") AND ("alignment" OR "in line with" OR "geared to" OR "aligned with" OR "linking") AND ("method" OR "approach" OR "framework" OR "methodology")) AND PUBYEAR &lt; 2016 </t>
   </si>
   <si>
-    <t>3 são proceeding de conferencia</t>
-  </si>
-  <si>
     <t>11 estavam repetidos e 2 estavam sem autor.</t>
   </si>
   <si>
@@ -973,12 +968,57 @@
     <t>RQ2.1)A estratégia envolve analisar menos artigos quando comparada com as SLRs publicadas que conduziram buscas somente em bases de dados? Precision
 RQ2.2)A estratégia recupera todos os artigos que estavam incluídos na SLR publicada que conduziu as buscas em bases de dados? Recall.</t>
   </si>
+  <si>
+    <t>337 mas limitado a Subdiscipline = Software Engineering and pub year 2015, temos 141</t>
+  </si>
+  <si>
+    <t>141 mas limitado a ACM temos 109.</t>
+  </si>
+  <si>
+    <t>2/22=9%</t>
+  </si>
+  <si>
+    <t>2/26= 7,6%</t>
+  </si>
+  <si>
+    <t>Alterar a estrategias guideline e short paper para primeiro executar backward.</t>
+  </si>
+  <si>
+    <t>Incluídos com o aliases - buscar com JF e remover</t>
+  </si>
+  <si>
+    <t>Utilizei a mesma query do IEEE (reduzida)</t>
+  </si>
+  <si>
+    <t>Limitado a 2015</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com.br/scholar?q=%28%28%22software+process+improvement%22%29+AND+%28%22business+goal%22%29+AND+%28%22alignment%22+OR+%22in+line+with%22%29+AND+%28%22method%22+OR+%22approach%22%29%29&amp;hl=pt-BR&amp;as_sdt=0%2C5&amp;as_ylo=&amp;as_yhi=2015</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>4/40= 10%</t>
+  </si>
+  <si>
+    <t>4/22= 18%</t>
+  </si>
+  <si>
+    <t>(Google Scholar para Guideline)</t>
+  </si>
+  <si>
+    <t>Duas páginas, cada uma com 20 resultados, organizados por relevância</t>
+  </si>
+  <si>
+    <t>3 são proceeding de conferencia.Nas evidências de Vasc. temos 18</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1052,8 +1092,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1168,6 +1215,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -1532,11 +1585,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1631,7 +1685,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1806,6 +1859,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1857,6 +1928,9 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1908,20 +1982,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2201,7 +2281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -2212,107 +2292,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="114" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="115"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="108"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="B2" s="117"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="110"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="109" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="110"/>
+      <c r="B3" s="117"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>101</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="111" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="112"/>
+      <c r="B8" s="119"/>
     </row>
     <row r="9" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>118</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2345,10 +2425,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="118"/>
+      <c r="A1" s="124" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="125"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
@@ -2363,7 +2443,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2374,23 +2454,23 @@
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="113" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="114"/>
+      <c r="A6" s="120" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="121"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="115" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" s="116"/>
+      <c r="A7" s="122" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="123"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
@@ -2452,391 +2532,381 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" style="16" customWidth="1"/>
+    <col min="2" max="2" width="17" style="16" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="16" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="41.7109375" style="16" customWidth="1"/>
-    <col min="8" max="8" width="54.28515625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="53.5703125" style="16" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="16"/>
+    <col min="6" max="6" width="41.7109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="54.28515625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" style="16" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="121"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="126" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="128"/>
+      <c r="J1" s="16"/>
       <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="F2" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="77">
+        <v>15</v>
+      </c>
+      <c r="C3" s="44">
+        <v>20</v>
+      </c>
+      <c r="D3" s="77" t="s">
+        <v>300</v>
+      </c>
+      <c r="E3" s="44">
+        <v>17</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="44">
+        <v>10</v>
+      </c>
+      <c r="C4" s="44">
+        <v>10</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44">
+        <v>10</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="44">
+        <v>13</v>
+      </c>
+      <c r="C5" s="44">
+        <v>20</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="44">
+        <v>16</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="49">
+        <v>100</v>
+      </c>
+      <c r="C6" s="110" t="s">
+        <v>287</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="49">
+        <v>103</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="44">
+        <v>43</v>
+      </c>
+      <c r="C7" s="44">
+        <v>26</v>
+      </c>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44">
+        <v>26</v>
+      </c>
+      <c r="F7" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="G7" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="49">
+        <v>141</v>
+      </c>
+      <c r="C8" s="110" t="s">
+        <v>286</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="49">
+        <v>128</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="44">
+        <v>195</v>
+      </c>
+      <c r="C9" s="44">
+        <v>189</v>
+      </c>
+      <c r="D9" s="77" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="44">
+        <v>182</v>
+      </c>
+      <c r="F9" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="H9" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-    </row>
-    <row r="3" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="45">
-        <v>15</v>
-      </c>
-      <c r="C3" s="50">
-        <v>20</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="E3" s="45">
-        <v>17</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>161</v>
-      </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-    </row>
-    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="45">
-        <v>10</v>
-      </c>
-      <c r="C4" s="50">
-        <v>10</v>
-      </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45">
-        <v>10</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H4" s="49" t="s">
-        <v>173</v>
-      </c>
-      <c r="I4" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-    </row>
-    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="45">
-        <v>13</v>
-      </c>
-      <c r="C5" s="50">
-        <v>20</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>164</v>
-      </c>
-      <c r="E5" s="45">
-        <v>16</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="H5" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-    </row>
-    <row r="6" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="45">
-        <v>100</v>
-      </c>
-      <c r="C6" s="45">
-        <v>141</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" s="45">
-        <v>103</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="I6" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="45">
-        <v>43</v>
-      </c>
-      <c r="C7" s="45">
-        <v>26</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45">
-        <v>26</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="I7" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="45">
-        <v>141</v>
-      </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="E8" s="45">
-        <v>128</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="47" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="49" t="s">
-        <v>177</v>
-      </c>
-      <c r="I8" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-    </row>
-    <row r="9" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="45">
-        <v>195</v>
-      </c>
-      <c r="C9" s="45">
-        <v>189</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>166</v>
-      </c>
-      <c r="E9" s="45">
-        <v>182</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="H9" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="I9" s="47" t="s">
-        <v>156</v>
-      </c>
+      <c r="J9" s="16"/>
       <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
-      <c r="B10" s="11">
+      <c r="B10" s="155">
         <f>SUM(B3:B9)</f>
         <v>517</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="E10" s="11">
+      <c r="C10" s="155"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="155">
         <f>SUM(E3:E9)</f>
         <v>482</v>
       </c>
-      <c r="F10" s="44"/>
+      <c r="J10" s="16"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="16"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="16"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="16"/>
       <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="16"/>
       <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="16"/>
       <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="16"/>
       <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-    </row>
-    <row r="17" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="16"/>
       <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-    </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="16"/>
       <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-    </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="16"/>
       <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-    </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="16"/>
       <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="16"/>
       <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-    </row>
-    <row r="22" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="16"/>
       <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-    </row>
-    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="16"/>
       <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-    </row>
-    <row r="24" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="16"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-    </row>
-    <row r="25" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="16"/>
       <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-    </row>
-    <row r="26" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="16"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-    </row>
-    <row r="27" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="16"/>
       <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-    </row>
-    <row r="28" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="16"/>
       <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-    </row>
-    <row r="29" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="16"/>
       <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-    </row>
-    <row r="30" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="16"/>
       <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-    </row>
-    <row r="31" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="16"/>
       <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-    </row>
-    <row r="32" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J32" s="16"/>
       <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-    </row>
-    <row r="33" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="16"/>
       <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-    </row>
-    <row r="34" spans="11:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="16"/>
       <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H7" display="http://ieeexplore.ieee.org/search/searchresult.jsp?action=search&amp;matchBoolean=true&amp;searchField=Search_All_Text&amp;queryText=(((.QT.software%20process%20improvement.QT.)%20AND%20(.QT.business%20goal.QT.)%20AND%20(.QT.alignment.QT.%20OR%20.QT.in%20line%20with."/>
-    <hyperlink ref="H6" display="https://dl.acm.org/results.cfm?query=%252B(%22software%20process%20improvement%22%20%252B(%22business%20goal%22%20%22strategic%22%20%22goal%20oriented%22%20%22business%20oriented%22%20%22business%20strategy%22)%20%252B(%22alignment%22%20%22in%20line%20wit"/>
-    <hyperlink ref="H4" r:id="rId1"/>
-    <hyperlink ref="H8" display="https://link.springer.com/search?query=%22software+process+improvement%22+and+%28%22business+goal%22+or+%22strategic%22+or+%22goal+oriented%22+or+%22business+oriented%22+or+%22business+strategy%22%29+and+%28%22alignment%22+or++%22in+line+with%22+or+%22gea"/>
-    <hyperlink ref="H9" r:id="rId2"/>
-    <hyperlink ref="H5" r:id="rId3"/>
+    <hyperlink ref="G7" display="http://ieeexplore.ieee.org/search/searchresult.jsp?action=search&amp;matchBoolean=true&amp;searchField=Search_All_Text&amp;queryText=(((.QT.software%20process%20improvement.QT.)%20AND%20(.QT.business%20goal.QT.)%20AND%20(.QT.alignment.QT.%20OR%20.QT.in%20line%20with."/>
+    <hyperlink ref="G6" display="https://dl.acm.org/results.cfm?query=%252B(%22software%20process%20improvement%22%20%252B(%22business%20goal%22%20%22strategic%22%20%22goal%20oriented%22%20%22business%20oriented%22%20%22business%20strategy%22)%20%252B(%22alignment%22%20%22in%20line%20wit"/>
+    <hyperlink ref="G4" r:id="rId1"/>
+    <hyperlink ref="G8" display="https://link.springer.com/search?query=%22software+process+improvement%22+and+%28%22business+goal%22+or+%22strategic%22+or+%22goal+oriented%22+or+%22business+oriented%22+or+%22business+strategy%22%29+and+%28%22alignment%22+or++%22in+line+with%22+or+%22gea"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2862,406 +2932,406 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
+      <c r="A1" s="129" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
     </row>
     <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="E2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>38</v>
-      </c>
       <c r="F2" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="G2" s="105" t="s">
-        <v>248</v>
+        <v>147</v>
+      </c>
+      <c r="G2" s="104" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="26" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>27</v>
       </c>
       <c r="F3" s="7">
         <v>25</v>
       </c>
-      <c r="G3" s="70"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="10">
         <v>2007</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F4" s="7">
         <v>20</v>
       </c>
-      <c r="G4" s="95">
+      <c r="G4" s="94">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="10">
         <v>2008</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F5" s="7">
         <v>24</v>
       </c>
-      <c r="G5" s="95">
+      <c r="G5" s="94">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>33</v>
       </c>
       <c r="D6" s="10">
         <v>2015</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F6" s="7">
         <v>57</v>
       </c>
-      <c r="G6" s="95"/>
+      <c r="G6" s="94"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="D7" s="10">
         <v>2011</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="5">
         <v>11</v>
       </c>
-      <c r="G7" s="73">
+      <c r="G7" s="72">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>60</v>
       </c>
       <c r="D8" s="10">
         <v>2010</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="5">
         <v>22</v>
       </c>
-      <c r="G8" s="73"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D9" s="10">
         <v>2009</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="5">
         <v>13</v>
       </c>
-      <c r="G9" s="70"/>
+      <c r="G9" s="69"/>
     </row>
     <row r="10" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="10">
         <v>2010</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10" s="5">
         <v>43</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G10" s="72">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D11" s="10">
         <v>2010</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F11" s="5">
         <v>11</v>
       </c>
-      <c r="G11" s="70"/>
+      <c r="G11" s="69"/>
     </row>
     <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="10">
         <v>1999</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" s="6">
         <v>37</v>
       </c>
-      <c r="G12" s="70"/>
+      <c r="G12" s="69"/>
     </row>
     <row r="13" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>69</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>70</v>
       </c>
       <c r="D13" s="10">
         <v>2005</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F13" s="5">
         <v>16</v>
       </c>
-      <c r="G13" s="70"/>
+      <c r="G13" s="69"/>
     </row>
     <row r="14" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D14" s="10">
         <v>2008</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" s="5">
         <v>14</v>
       </c>
-      <c r="G14" s="73">
+      <c r="G14" s="72">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>73</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>74</v>
       </c>
       <c r="D15" s="10">
         <v>2011</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F15" s="5">
         <v>8</v>
       </c>
-      <c r="G15" s="73">
+      <c r="G15" s="72">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>75</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>76</v>
       </c>
       <c r="D16" s="10">
         <v>2009</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" s="5">
         <v>27</v>
       </c>
-      <c r="G16" s="73">
+      <c r="G16" s="72">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="10">
         <v>1997</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F17" s="5">
         <v>14</v>
       </c>
-      <c r="G17" s="73">
+      <c r="G17" s="72">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>79</v>
       </c>
       <c r="D18" s="10">
         <v>2010</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F18" s="5">
         <v>8</v>
       </c>
-      <c r="G18" s="70"/>
+      <c r="G18" s="69"/>
     </row>
     <row r="19" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D19" s="10">
         <v>2005</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F19" s="5">
         <v>15</v>
@@ -3270,19 +3340,19 @@
     </row>
     <row r="20" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>83</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>84</v>
       </c>
       <c r="D20" s="10">
         <v>2011</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F20" s="5">
         <v>18</v>
@@ -3291,40 +3361,40 @@
     </row>
     <row r="21" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>85</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>86</v>
       </c>
       <c r="D21" s="10">
         <v>2008</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F21" s="5">
         <v>22</v>
       </c>
-      <c r="G21" s="70"/>
+      <c r="G21" s="69"/>
     </row>
     <row r="22" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>87</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>88</v>
       </c>
       <c r="D22" s="10">
         <v>2015</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F22" s="5">
         <v>15</v>
@@ -3333,65 +3403,65 @@
     </row>
     <row r="23" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>89</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>90</v>
       </c>
       <c r="D23" s="10">
         <v>2000</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F23" s="5">
         <v>11</v>
       </c>
-      <c r="G23" s="70"/>
+      <c r="G23" s="69"/>
     </row>
     <row r="24" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="26" t="s">
         <v>92</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>93</v>
       </c>
       <c r="D24" s="10">
         <v>2010</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F24" s="5">
         <v>33</v>
       </c>
-      <c r="G24" s="70"/>
+      <c r="G24" s="69"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E25" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F25" s="9">
         <f>SUM(F3:F24)</f>
         <v>464</v>
       </c>
-      <c r="G25" s="70">
+      <c r="G25" s="69">
         <f>SUM(G3:G24)</f>
         <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3407,10 +3477,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3422,89 +3492,89 @@
     <col min="5" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
-        <v>253</v>
-      </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
+    <row r="1" spans="1:19" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="137" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="141" t="s">
-        <v>252</v>
-      </c>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
+      <c r="A2" s="131" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="123" t="s">
-        <v>251</v>
-      </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="106"/>
-      <c r="L3" s="106"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="106"/>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
+      <c r="A3" s="130" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="105"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="128" t="s">
-        <v>276</v>
-      </c>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-    </row>
-    <row r="5" spans="1:19" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
-        <v>244</v>
-      </c>
-      <c r="B5" s="98" t="s">
-        <v>210</v>
-      </c>
-      <c r="C5" s="98" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" s="98" t="s">
-        <v>273</v>
+      <c r="A4" s="136" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="136"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+    </row>
+    <row r="5" spans="1:19" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="97" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" s="97" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="97" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="97" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="C6" s="74" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" s="124" t="s">
-        <v>274</v>
+      <c r="B6" s="73" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" s="132" t="s">
+        <v>272</v>
       </c>
       <c r="N6" s="38"/>
     </row>
@@ -3512,359 +3582,383 @@
       <c r="A7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="C7" s="74" t="s">
-        <v>250</v>
-      </c>
-      <c r="D7" s="125"/>
+      <c r="B7" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" s="133"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="74" t="s">
-        <v>254</v>
-      </c>
-      <c r="C8" s="74" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="125"/>
+      <c r="B8" s="73" t="s">
+        <v>252</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" s="133"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="74" t="s">
-        <v>255</v>
-      </c>
-      <c r="C9" s="74" t="s">
-        <v>259</v>
-      </c>
-      <c r="D9" s="125"/>
+      <c r="B9" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>257</v>
+      </c>
+      <c r="D9" s="133"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="C10" s="74" t="s">
-        <v>260</v>
-      </c>
-      <c r="D10" s="125"/>
+      <c r="B10" s="73" t="s">
+        <v>254</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="133"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="C11" s="74" t="s">
-        <v>260</v>
-      </c>
-      <c r="D11" s="125"/>
+      <c r="B11" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="133"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="126"/>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="141" t="s">
+      <c r="B12" s="73" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" s="134"/>
+    </row>
+    <row r="13" spans="1:19" s="151" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="150" t="s">
+        <v>298</v>
+      </c>
+      <c r="B13" s="73" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="109"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="131" t="s">
+        <v>282</v>
+      </c>
+      <c r="B14" s="131"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="131"/>
+      <c r="I14" s="131"/>
+    </row>
+    <row r="15" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="130" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" s="130"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="105"/>
+      <c r="O15" s="105"/>
+      <c r="P15" s="105"/>
+      <c r="Q15" s="105"/>
+      <c r="R15" s="105"/>
+      <c r="S15" s="105"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="135" t="s">
+        <v>280</v>
+      </c>
+      <c r="B16" s="136"/>
+      <c r="C16" s="136"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="136"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="97" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17" s="97" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" s="97" t="s">
+        <v>270</v>
+      </c>
+      <c r="D17" s="97" t="s">
+        <v>271</v>
+      </c>
+      <c r="E17" s="97" t="s">
+        <v>208</v>
+      </c>
+      <c r="F17" s="97" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="108" t="s">
+        <v>273</v>
+      </c>
+      <c r="B18" s="69" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="D18" s="73" t="s">
+        <v>279</v>
+      </c>
+      <c r="E18" s="107">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F18" s="106">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="108" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" s="69" t="s">
+        <v>262</v>
+      </c>
+      <c r="C19" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="D19" s="73" t="s">
+        <v>264</v>
+      </c>
+      <c r="E19" s="149">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F19" s="106">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="108" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="69" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>265</v>
+      </c>
+      <c r="E20" s="107">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F20" s="106">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="108" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="69" t="s">
+        <v>263</v>
+      </c>
+      <c r="C21" s="73" t="s">
+        <v>276</v>
+      </c>
+      <c r="D21" s="73" t="s">
+        <v>266</v>
+      </c>
+      <c r="E21" s="107">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F21" s="106">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="108" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="69" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>277</v>
+      </c>
+      <c r="D22" s="73" t="s">
+        <v>267</v>
+      </c>
+      <c r="E22" s="107">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F22" s="106">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="108" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="69" t="s">
         <v>284</v>
       </c>
-      <c r="B13" s="141"/>
-      <c r="C13" s="141"/>
-      <c r="D13" s="141"/>
-      <c r="E13" s="141"/>
-      <c r="F13" s="141"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="141"/>
-      <c r="I13" s="141"/>
-    </row>
-    <row r="14" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="123" t="s">
-        <v>261</v>
-      </c>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="123"/>
-      <c r="J14" s="106"/>
-      <c r="K14" s="106"/>
-      <c r="L14" s="106"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="106"/>
-      <c r="O14" s="106"/>
-      <c r="P14" s="106"/>
-      <c r="Q14" s="106"/>
-      <c r="R14" s="106"/>
-      <c r="S14" s="106"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="127" t="s">
-        <v>282</v>
-      </c>
-      <c r="B15" s="128"/>
-      <c r="C15" s="128"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="F15" s="128"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="98" t="s">
-        <v>262</v>
-      </c>
-      <c r="B16" s="98" t="s">
-        <v>263</v>
-      </c>
-      <c r="C16" s="98" t="s">
+      <c r="C23" s="73" t="s">
+        <v>278</v>
+      </c>
+      <c r="D23" s="73" t="s">
+        <v>268</v>
+      </c>
+      <c r="E23" s="107">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="F23" s="106">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="131" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" s="131"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="131"/>
+      <c r="G24" s="131"/>
+      <c r="H24" s="131"/>
+      <c r="I24" s="131"/>
+    </row>
+    <row r="25" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="130" t="s">
+        <v>285</v>
+      </c>
+      <c r="B25" s="130"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="97" t="s">
+        <v>271</v>
+      </c>
+      <c r="B26" s="97" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26" s="97" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="76" t="s">
         <v>272</v>
       </c>
-      <c r="D16" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="E16" s="98" t="s">
-        <v>210</v>
-      </c>
-      <c r="F16" s="98" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="144" t="s">
-        <v>275</v>
-      </c>
-      <c r="B17" s="70" t="s">
+      <c r="B27" s="107">
+        <v>0.47</v>
+      </c>
+      <c r="C27" s="106">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="76" t="s">
+        <v>279</v>
+      </c>
+      <c r="B28" s="107">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C28" s="106">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="C17" s="74" t="s">
-        <v>277</v>
-      </c>
-      <c r="D17" s="74" t="s">
-        <v>281</v>
-      </c>
-      <c r="E17" s="143">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F17" s="142">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="144" t="s">
-        <v>271</v>
-      </c>
-      <c r="B18" s="70" t="s">
-        <v>264</v>
-      </c>
-      <c r="C18" s="74" t="s">
-        <v>277</v>
-      </c>
-      <c r="D18" s="74" t="s">
+      <c r="B29" s="149">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C29" s="106">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="76" t="s">
+        <v>265</v>
+      </c>
+      <c r="B30" s="107">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C30" s="106">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="76" t="s">
         <v>266</v>
       </c>
-      <c r="E18" s="142"/>
-      <c r="F18" s="142"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="144" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="70" t="s">
-        <v>264</v>
-      </c>
-      <c r="C19" s="74" t="s">
-        <v>277</v>
-      </c>
-      <c r="D19" s="74" t="s">
+      <c r="B31" s="107">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="C31" s="106">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="76" t="s">
         <v>267</v>
       </c>
-      <c r="E19" s="143">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F19" s="142">
+      <c r="B32" s="107">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C32" s="106">
         <v>0.59</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="144" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="70" t="s">
-        <v>265</v>
-      </c>
-      <c r="C20" s="74" t="s">
-        <v>278</v>
-      </c>
-      <c r="D20" s="74" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="76" t="s">
         <v>268</v>
       </c>
-      <c r="E20" s="143">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="F20" s="142">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="144" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="70" t="s">
-        <v>285</v>
-      </c>
-      <c r="C21" s="74" t="s">
-        <v>279</v>
-      </c>
-      <c r="D21" s="74" t="s">
-        <v>269</v>
-      </c>
-      <c r="E21" s="143">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="F21" s="142">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="144" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="70" t="s">
-        <v>286</v>
-      </c>
-      <c r="C22" s="74" t="s">
-        <v>280</v>
-      </c>
-      <c r="D22" s="74" t="s">
-        <v>270</v>
-      </c>
-      <c r="E22" s="143">
+      <c r="B33" s="107">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="F22" s="142">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="141" t="s">
-        <v>283</v>
-      </c>
-      <c r="B23" s="141"/>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
-    </row>
-    <row r="24" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="123" t="s">
-        <v>287</v>
-      </c>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="123"/>
-      <c r="G24" s="123"/>
-      <c r="H24" s="123"/>
-      <c r="I24" s="123"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B25" s="98" t="s">
-        <v>210</v>
-      </c>
-      <c r="C25" s="98" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="77" t="s">
-        <v>274</v>
-      </c>
-      <c r="B26" s="142">
-        <v>0.47</v>
-      </c>
-      <c r="C26" s="142">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="77" t="s">
-        <v>281</v>
-      </c>
-      <c r="B27" s="143">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C27" s="142">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="77" t="s">
-        <v>266</v>
-      </c>
-      <c r="B28" s="142"/>
-      <c r="C28" s="142"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="77" t="s">
-        <v>267</v>
-      </c>
-      <c r="B29" s="143">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="C29" s="142">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="77" t="s">
-        <v>268</v>
-      </c>
-      <c r="B30" s="143">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="C30" s="142">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="77" t="s">
-        <v>269</v>
-      </c>
-      <c r="B31" s="143">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="C31" s="142">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="77" t="s">
-        <v>270</v>
-      </c>
-      <c r="B32" s="143">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="C32" s="142">
+      <c r="C33" s="106">
         <v>0.54</v>
       </c>
     </row>
@@ -3874,12 +3968,12 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A23:I23"/>
     <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A25:I25"/>
     <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:I15"/>
     <mergeCell ref="D6:D12"/>
-    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3908,737 +4002,737 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
+      <c r="A1" s="144" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
     </row>
     <row r="2" spans="1:14" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
+      <c r="A2" s="141" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="142"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="148" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="148"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="148"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="C4" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="D4" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="E4" s="71" t="s">
         <v>184</v>
       </c>
-      <c r="D4" s="72" t="s">
-        <v>185</v>
-      </c>
-      <c r="E4" s="72" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="72" t="s">
+      <c r="F4" s="71" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" s="71" t="s">
+        <v>241</v>
+      </c>
+      <c r="H4" s="71" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="73"/>
+    </row>
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73">
+        <v>20</v>
+      </c>
+      <c r="G6" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="102" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="51" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="52"/>
+      <c r="C7" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73">
+        <v>24</v>
+      </c>
+      <c r="G7" s="101" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="103" t="s">
         <v>220</v>
       </c>
-      <c r="G4" s="72" t="s">
-        <v>243</v>
-      </c>
-      <c r="H4" s="72" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="92" t="s">
+    </row>
+    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="52"/>
+      <c r="C8" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="78" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="74"/>
-    </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="101" t="s">
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="73"/>
+    </row>
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="52"/>
+      <c r="C9" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74">
-        <v>20</v>
-      </c>
-      <c r="G6" s="102" t="s">
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73">
+        <v>11</v>
+      </c>
+      <c r="G9" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="102" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="73"/>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="52"/>
+      <c r="C11" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="73"/>
+    </row>
+    <row r="12" spans="1:14" s="51" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="98">
+        <v>44</v>
+      </c>
+      <c r="G12" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="102" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="73"/>
+    </row>
+    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="73"/>
+    </row>
+    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="73"/>
+    </row>
+    <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="52"/>
+      <c r="C16" s="100" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73">
         <v>14</v>
       </c>
-      <c r="H6" s="103" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="101" t="s">
+      <c r="G16" s="101" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="102" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="51" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="52"/>
+      <c r="C17" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74">
-        <v>24</v>
-      </c>
-      <c r="G7" s="102" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="104" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="92" t="s">
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73">
+        <v>8</v>
+      </c>
+      <c r="G17" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="102" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="52"/>
+      <c r="C18" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="74"/>
-    </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="101" t="s">
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73">
+        <v>27</v>
+      </c>
+      <c r="G18" s="101" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="102" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="51" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="52"/>
+      <c r="C19" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74">
-        <v>11</v>
-      </c>
-      <c r="G9" s="102" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="103" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="92" t="s">
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73">
+        <v>14</v>
+      </c>
+      <c r="G19" s="101" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="102" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="52"/>
+      <c r="C20" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="74"/>
-    </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="92" t="s">
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="73"/>
+    </row>
+    <row r="21" spans="1:11" s="51" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="52"/>
+      <c r="C21" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="74"/>
-    </row>
-    <row r="12" spans="1:14" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="101" t="s">
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="73"/>
+    </row>
+    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="52"/>
+      <c r="C22" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="99">
-        <v>44</v>
-      </c>
-      <c r="G12" s="102" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="103" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="92" t="s">
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="73"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="52"/>
+      <c r="C23" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="74"/>
-    </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="92" t="s">
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="77" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="73"/>
+    </row>
+    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="52"/>
+      <c r="C24" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="74"/>
-    </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="92" t="s">
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="73"/>
+    </row>
+    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="52"/>
+      <c r="C25" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="74"/>
-    </row>
-    <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="101" t="s">
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="73"/>
+    </row>
+    <row r="26" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="52"/>
+      <c r="C26" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74">
-        <v>14</v>
-      </c>
-      <c r="G16" s="102" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="103" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74">
-        <v>8</v>
-      </c>
-      <c r="G17" s="102" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="103" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74">
-        <v>27</v>
-      </c>
-      <c r="G18" s="102" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="103" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74">
-        <v>14</v>
-      </c>
-      <c r="G19" s="102" t="s">
-        <v>77</v>
-      </c>
-      <c r="H19" s="103" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="92" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="H20" s="74"/>
-    </row>
-    <row r="21" spans="1:11" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="92" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" s="74"/>
-    </row>
-    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="92" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="78" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" s="74"/>
-    </row>
-    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="92" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="78" t="s">
-        <v>85</v>
-      </c>
-      <c r="H23" s="74"/>
-    </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="53"/>
-      <c r="C24" s="92" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="78" t="s">
-        <v>87</v>
-      </c>
-      <c r="H24" s="74"/>
-    </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="92" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="78" t="s">
-        <v>89</v>
-      </c>
-      <c r="H25" s="74"/>
-    </row>
-    <row r="26" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="92" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="78" t="s">
-        <v>92</v>
-      </c>
-      <c r="H26" s="74"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" s="73"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="74"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="100">
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="99">
         <f>SUM(F5:F26)</f>
         <v>162</v>
       </c>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-    </row>
-    <row r="28" spans="1:11" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F28" s="75"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+    </row>
+    <row r="28" spans="1:11" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="74"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="138" t="s">
+      <c r="A29" s="146" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="146"/>
+      <c r="C29" s="146"/>
+      <c r="D29" s="67"/>
+      <c r="I29" s="145" t="s">
+        <v>203</v>
+      </c>
+      <c r="J29" s="145"/>
+      <c r="K29" s="145"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="147" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="147"/>
+      <c r="C30" s="73" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="70"/>
+      <c r="I30" s="76" t="s">
+        <v>204</v>
+      </c>
+      <c r="J30" s="73">
+        <v>17</v>
+      </c>
+      <c r="K30" s="85"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="147" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="147"/>
+      <c r="C31" s="81" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" s="70"/>
+      <c r="I31" s="76" t="s">
+        <v>205</v>
+      </c>
+      <c r="J31" s="73">
+        <v>22</v>
+      </c>
+      <c r="K31" s="72"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="147" t="s">
         <v>189</v>
       </c>
-      <c r="B29" s="138"/>
-      <c r="C29" s="138"/>
-      <c r="D29" s="68"/>
-      <c r="I29" s="137" t="s">
-        <v>205</v>
-      </c>
-      <c r="J29" s="137"/>
-      <c r="K29" s="137"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="139" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="139"/>
-      <c r="C30" s="74" t="s">
-        <v>204</v>
-      </c>
-      <c r="D30" s="71"/>
-      <c r="I30" s="77" t="s">
+      <c r="B32" s="147"/>
+      <c r="C32" s="81" t="s">
+        <v>238</v>
+      </c>
+      <c r="D32" s="70"/>
+      <c r="I32" s="83" t="s">
+        <v>216</v>
+      </c>
+      <c r="J32" s="72">
+        <v>8</v>
+      </c>
+      <c r="K32" s="72"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="139" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="139"/>
+      <c r="C33" s="140" t="s">
+        <v>229</v>
+      </c>
+      <c r="D33" s="96"/>
+      <c r="I33" s="83" t="s">
         <v>206</v>
       </c>
-      <c r="J30" s="74">
-        <v>17</v>
-      </c>
-      <c r="K30" s="86"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="139" t="s">
-        <v>190</v>
-      </c>
-      <c r="B31" s="139"/>
-      <c r="C31" s="82" t="s">
+      <c r="J33" s="72">
+        <v>14</v>
+      </c>
+      <c r="K33" s="72"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="139"/>
+      <c r="B34" s="139"/>
+      <c r="C34" s="140"/>
+      <c r="D34" s="96"/>
+      <c r="I34" s="82" t="s">
+        <v>183</v>
+      </c>
+      <c r="J34" s="86" t="s">
+        <v>235</v>
+      </c>
+      <c r="K34" s="73"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I35" s="82" t="s">
+        <v>184</v>
+      </c>
+      <c r="J35" s="86" t="s">
+        <v>236</v>
+      </c>
+      <c r="K35" s="73"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I36" s="84"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="75"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I37" s="79" t="s">
+        <v>207</v>
+      </c>
+      <c r="J37" s="78" t="s">
+        <v>208</v>
+      </c>
+      <c r="K37" s="78" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I38" s="91" t="s">
+        <v>210</v>
+      </c>
+      <c r="J38" s="77" t="s">
+        <v>217</v>
+      </c>
+      <c r="K38" s="80" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I39" s="90" t="s">
+        <v>211</v>
+      </c>
+      <c r="J39" s="86" t="s">
+        <v>234</v>
+      </c>
+      <c r="K39" s="81" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I40" s="90" t="s">
+        <v>212</v>
+      </c>
+      <c r="J40" s="86" t="s">
+        <v>228</v>
+      </c>
+      <c r="K40" s="81" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I41" s="89" t="s">
+        <v>214</v>
+      </c>
+      <c r="J41" s="87" t="s">
+        <v>233</v>
+      </c>
+      <c r="K41" s="81" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I42" s="92" t="s">
+        <v>215</v>
+      </c>
+      <c r="J42" s="88" t="s">
         <v>239</v>
       </c>
-      <c r="D31" s="71"/>
-      <c r="I31" s="77" t="s">
-        <v>207</v>
-      </c>
-      <c r="J31" s="74">
-        <v>22</v>
-      </c>
-      <c r="K31" s="73"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="139" t="s">
-        <v>191</v>
-      </c>
-      <c r="B32" s="139"/>
-      <c r="C32" s="82" t="s">
+      <c r="K42" s="73" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="I44" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="J44" s="95" t="s">
         <v>240</v>
-      </c>
-      <c r="D32" s="71"/>
-      <c r="I32" s="84" t="s">
-        <v>218</v>
-      </c>
-      <c r="J32" s="73">
-        <v>8</v>
-      </c>
-      <c r="K32" s="73"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="131" t="s">
-        <v>192</v>
-      </c>
-      <c r="B33" s="131"/>
-      <c r="C33" s="132" t="s">
-        <v>231</v>
-      </c>
-      <c r="D33" s="97"/>
-      <c r="I33" s="84" t="s">
-        <v>208</v>
-      </c>
-      <c r="J33" s="73">
-        <v>14</v>
-      </c>
-      <c r="K33" s="73"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="131"/>
-      <c r="B34" s="131"/>
-      <c r="C34" s="132"/>
-      <c r="D34" s="97"/>
-      <c r="I34" s="83" t="s">
-        <v>185</v>
-      </c>
-      <c r="J34" s="87" t="s">
-        <v>237</v>
-      </c>
-      <c r="K34" s="74"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I35" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="J35" s="87" t="s">
-        <v>238</v>
-      </c>
-      <c r="K35" s="74"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I36" s="85"/>
-      <c r="J36" s="76"/>
-      <c r="K36" s="76"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I37" s="80" t="s">
-        <v>209</v>
-      </c>
-      <c r="J37" s="79" t="s">
-        <v>210</v>
-      </c>
-      <c r="K37" s="79" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I38" s="92" t="s">
-        <v>212</v>
-      </c>
-      <c r="J38" s="78" t="s">
-        <v>219</v>
-      </c>
-      <c r="K38" s="81" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I39" s="91" t="s">
-        <v>213</v>
-      </c>
-      <c r="J39" s="87" t="s">
-        <v>236</v>
-      </c>
-      <c r="K39" s="82" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I40" s="91" t="s">
-        <v>214</v>
-      </c>
-      <c r="J40" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="K40" s="82" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I41" s="90" t="s">
-        <v>216</v>
-      </c>
-      <c r="J41" s="88" t="s">
-        <v>235</v>
-      </c>
-      <c r="K41" s="82" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I42" s="93" t="s">
-        <v>217</v>
-      </c>
-      <c r="J42" s="89" t="s">
-        <v>241</v>
-      </c>
-      <c r="K42" s="74" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="I44" s="94" t="s">
-        <v>232</v>
-      </c>
-      <c r="J44" s="96" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I47" s="62" t="s">
+      <c r="I47" s="61" t="s">
+        <v>191</v>
+      </c>
+      <c r="J47" s="53" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I48" s="62" t="s">
         <v>193</v>
       </c>
-      <c r="J47" s="54" t="s">
+      <c r="J48" s="54">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="63" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I48" s="63" t="s">
+      <c r="J49" s="55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="62" t="s">
         <v>195</v>
       </c>
-      <c r="J48" s="55">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I49" s="64" t="s">
+      <c r="J50" s="54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="J49" s="56">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I50" s="63" t="s">
+      <c r="J51" s="55" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="J50" s="55">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I51" s="64" t="s">
+      <c r="J52" s="56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="63" t="s">
         <v>198</v>
       </c>
-      <c r="J51" s="56" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I52" s="63" t="s">
+      <c r="J53" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="62" t="s">
         <v>199</v>
       </c>
-      <c r="J52" s="57">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I53" s="64" t="s">
+      <c r="J54" s="58"/>
+    </row>
+    <row r="55" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I55" s="64" t="s">
         <v>200</v>
       </c>
-      <c r="J53" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I54" s="63" t="s">
+      <c r="J55" s="59">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I56" s="65" t="s">
         <v>201</v>
       </c>
-      <c r="J54" s="59"/>
-    </row>
-    <row r="55" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I55" s="65" t="s">
-        <v>202</v>
-      </c>
-      <c r="J55" s="60">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I56" s="66" t="s">
-        <v>203</v>
-      </c>
-      <c r="J56" s="61">
+      <c r="J56" s="60">
         <v>12</v>
       </c>
     </row>
@@ -4662,7 +4756,61 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="154" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="112" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" s="113" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="153" t="s">
+        <v>295</v>
+      </c>
+      <c r="B3" s="72">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="152" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="152"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -4674,13 +4822,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>245</v>
+      <c r="A1" s="50" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
-        <v>246</v>
+      <c r="A4" s="93" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="111" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="111" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>